<commit_message>
GBDS DECEMBER FILES 2025 - fliqlo@GBDS
</commit_message>
<xml_diff>
--- a/GBDS DECEMBER FILES 2025/CSR MONTH OF DECEMBER.xlsx
+++ b/GBDS DECEMBER FILES 2025/CSR MONTH OF DECEMBER.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\GBDS DECEMBER FILES 2025\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7CF5E63-C3E5-49AE-B628-942510BA816F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0196AD61-4C0A-4EF7-8C66-92FB471054E4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="16" activeTab="28" xr2:uid="{67C3A74A-A57E-4AB5-8CD3-31B592A14032}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{67C3A74A-A57E-4AB5-8CD3-31B592A14032}"/>
   </bookViews>
   <sheets>
     <sheet name="CSR | DECEMBER" sheetId="902" r:id="rId1"/>
@@ -92,7 +92,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2352" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2367" uniqueCount="85">
   <si>
     <t>CHECKER STOCK REPORT</t>
   </si>
@@ -311,6 +311,42 @@
   </si>
   <si>
     <t>DATE ___________12/08/2025___________</t>
+  </si>
+  <si>
+    <t>5/1B</t>
+  </si>
+  <si>
+    <t>15/5B</t>
+  </si>
+  <si>
+    <t>20/6B</t>
+  </si>
+  <si>
+    <t>9/3B</t>
+  </si>
+  <si>
+    <t>3/1B</t>
+  </si>
+  <si>
+    <t>12/4B</t>
+  </si>
+  <si>
+    <t>12B</t>
+  </si>
+  <si>
+    <t>2/12B</t>
+  </si>
+  <si>
+    <t>1/12B</t>
+  </si>
+  <si>
+    <t>4/1B</t>
+  </si>
+  <si>
+    <t>7/12B</t>
+  </si>
+  <si>
+    <t>11/13B</t>
   </si>
 </sst>
 </file>
@@ -32435,7 +32471,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8327888C-2493-4ADD-8B4E-F904D8DF05AC}">
   <dimension ref="B1:AA43"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -33916,8 +33952,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD312018-AEFA-43EE-A4EC-98D8F1F0E5A4}">
   <dimension ref="B1:AA43"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
@@ -34271,11 +34307,19 @@
     <row r="8" spans="2:27" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="13"/>
       <c r="C8" s="14"/>
-      <c r="D8" s="15"/>
-      <c r="E8" s="15"/>
-      <c r="F8" s="15"/>
+      <c r="D8" s="15">
+        <v>3</v>
+      </c>
+      <c r="E8" s="15">
+        <v>1</v>
+      </c>
+      <c r="F8" s="15">
+        <v>1</v>
+      </c>
       <c r="G8" s="15"/>
-      <c r="H8" s="15"/>
+      <c r="H8" s="15" t="s">
+        <v>78</v>
+      </c>
       <c r="I8" s="15"/>
       <c r="J8" s="15"/>
       <c r="K8" s="15"/>
@@ -34287,9 +34331,13 @@
       <c r="Q8" s="15"/>
       <c r="R8" s="15"/>
       <c r="S8" s="15"/>
-      <c r="T8" s="15"/>
+      <c r="T8" s="15">
+        <v>2</v>
+      </c>
       <c r="U8" s="62"/>
-      <c r="V8" s="16"/>
+      <c r="V8" s="16">
+        <v>2</v>
+      </c>
     </row>
     <row r="9" spans="2:27" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="13" t="s">
@@ -34438,11 +34486,19 @@
         <v>25</v>
       </c>
       <c r="C15" s="23"/>
-      <c r="D15" s="24"/>
-      <c r="E15" s="24"/>
-      <c r="F15" s="24"/>
+      <c r="D15" s="24">
+        <v>0</v>
+      </c>
+      <c r="E15" s="24">
+        <v>0</v>
+      </c>
+      <c r="F15" s="24">
+        <v>0</v>
+      </c>
       <c r="G15" s="24"/>
-      <c r="H15" s="24"/>
+      <c r="H15" s="24" t="s">
+        <v>77</v>
+      </c>
       <c r="I15" s="24"/>
       <c r="J15" s="24"/>
       <c r="K15" s="24"/>
@@ -34454,20 +34510,32 @@
       <c r="Q15" s="24"/>
       <c r="R15" s="24"/>
       <c r="S15" s="24"/>
-      <c r="T15" s="24"/>
+      <c r="T15" s="24">
+        <v>1</v>
+      </c>
       <c r="U15" s="64"/>
-      <c r="V15" s="25"/>
+      <c r="V15" s="25">
+        <v>0</v>
+      </c>
     </row>
     <row r="16" spans="2:27" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B16" s="26" t="s">
         <v>26</v>
       </c>
       <c r="C16" s="60"/>
-      <c r="D16" s="61"/>
-      <c r="E16" s="28"/>
-      <c r="F16" s="28"/>
+      <c r="D16" s="61">
+        <v>3</v>
+      </c>
+      <c r="E16" s="28">
+        <v>1</v>
+      </c>
+      <c r="F16" s="28">
+        <v>1</v>
+      </c>
       <c r="G16" s="29"/>
-      <c r="H16" s="67"/>
+      <c r="H16" s="67" t="s">
+        <v>76</v>
+      </c>
       <c r="I16" s="29"/>
       <c r="J16" s="29"/>
       <c r="K16" s="59"/>
@@ -34479,9 +34547,13 @@
       <c r="Q16" s="29"/>
       <c r="R16" s="29"/>
       <c r="S16" s="29"/>
-      <c r="T16" s="59"/>
+      <c r="T16" s="59">
+        <v>1</v>
+      </c>
       <c r="U16" s="65"/>
-      <c r="V16" s="30"/>
+      <c r="V16" s="30">
+        <v>2</v>
+      </c>
     </row>
     <row r="17" spans="2:22" s="5" customFormat="1" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B17" s="31"/>
@@ -34859,21 +34931,37 @@
       <c r="B24" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="C24" s="14"/>
+      <c r="C24" s="14" t="s">
+        <v>79</v>
+      </c>
       <c r="D24" s="15"/>
-      <c r="E24" s="15"/>
+      <c r="E24" s="15">
+        <v>1</v>
+      </c>
       <c r="F24" s="15"/>
       <c r="G24" s="15"/>
-      <c r="H24" s="15"/>
+      <c r="H24" s="15" t="s">
+        <v>80</v>
+      </c>
       <c r="I24" s="15"/>
-      <c r="J24" s="15"/>
+      <c r="J24" s="15">
+        <v>20</v>
+      </c>
       <c r="K24" s="15"/>
-      <c r="L24" s="15"/>
-      <c r="M24" s="15"/>
-      <c r="N24" s="15"/>
+      <c r="L24" s="15">
+        <v>4</v>
+      </c>
+      <c r="M24" s="15">
+        <v>20</v>
+      </c>
+      <c r="N24" s="15">
+        <v>275</v>
+      </c>
       <c r="O24" s="15"/>
       <c r="P24" s="15"/>
-      <c r="Q24" s="15"/>
+      <c r="Q24" s="15">
+        <v>11</v>
+      </c>
       <c r="R24" s="15"/>
       <c r="S24" s="15"/>
       <c r="T24" s="15"/>
@@ -35024,21 +35112,37 @@
       <c r="B31" s="22" t="s">
         <v>25</v>
       </c>
-      <c r="C31" s="23"/>
+      <c r="C31" s="23">
+        <v>0</v>
+      </c>
       <c r="D31" s="24"/>
-      <c r="E31" s="24"/>
+      <c r="E31" s="24">
+        <v>1</v>
+      </c>
       <c r="F31" s="24"/>
       <c r="G31" s="24"/>
-      <c r="H31" s="24"/>
+      <c r="H31" s="24">
+        <v>0</v>
+      </c>
       <c r="I31" s="24"/>
-      <c r="J31" s="24"/>
+      <c r="J31" s="24">
+        <v>0</v>
+      </c>
       <c r="K31" s="24"/>
-      <c r="L31" s="24"/>
-      <c r="M31" s="24"/>
-      <c r="N31" s="24"/>
+      <c r="L31" s="24" t="s">
+        <v>80</v>
+      </c>
+      <c r="M31" s="24">
+        <v>4</v>
+      </c>
+      <c r="N31" s="24">
+        <v>13</v>
+      </c>
       <c r="O31" s="24"/>
       <c r="P31" s="24"/>
-      <c r="Q31" s="24"/>
+      <c r="Q31" s="24">
+        <v>0</v>
+      </c>
       <c r="R31" s="24"/>
       <c r="S31" s="24"/>
       <c r="T31" s="24"/>
@@ -35049,21 +35153,37 @@
       <c r="B32" s="39" t="s">
         <v>26</v>
       </c>
-      <c r="C32" s="27"/>
+      <c r="C32" s="27" t="s">
+        <v>79</v>
+      </c>
       <c r="D32" s="28"/>
-      <c r="E32" s="28"/>
+      <c r="E32" s="28">
+        <v>0</v>
+      </c>
       <c r="F32" s="28"/>
       <c r="G32" s="29"/>
-      <c r="H32" s="29"/>
+      <c r="H32" s="29" t="s">
+        <v>80</v>
+      </c>
       <c r="I32" s="29"/>
-      <c r="J32" s="29"/>
+      <c r="J32" s="29">
+        <v>20</v>
+      </c>
       <c r="K32" s="29"/>
-      <c r="L32" s="29"/>
-      <c r="M32" s="29"/>
-      <c r="N32" s="29"/>
+      <c r="L32" s="29" t="s">
+        <v>81</v>
+      </c>
+      <c r="M32" s="29">
+        <v>16</v>
+      </c>
+      <c r="N32" s="29">
+        <v>262</v>
+      </c>
       <c r="O32" s="24"/>
       <c r="P32" s="29"/>
-      <c r="Q32" s="29"/>
+      <c r="Q32" s="29">
+        <v>11</v>
+      </c>
       <c r="R32" s="29"/>
       <c r="S32" s="29"/>
       <c r="T32" s="29"/>
@@ -35189,21 +35309,51 @@
       <c r="B36" s="55" t="s">
         <v>52</v>
       </c>
-      <c r="C36" s="49"/>
-      <c r="D36" s="44"/>
-      <c r="E36" s="45"/>
-      <c r="F36" s="45"/>
-      <c r="G36" s="45"/>
-      <c r="H36" s="45"/>
-      <c r="I36" s="45"/>
-      <c r="J36" s="45"/>
-      <c r="K36" s="45"/>
-      <c r="L36" s="45"/>
-      <c r="M36" s="45"/>
-      <c r="N36" s="45"/>
-      <c r="O36" s="45"/>
-      <c r="P36" s="45"/>
-      <c r="Q36" s="46"/>
+      <c r="C36" s="49">
+        <v>1</v>
+      </c>
+      <c r="D36" s="44">
+        <v>2</v>
+      </c>
+      <c r="E36" s="45">
+        <v>1</v>
+      </c>
+      <c r="F36" s="45">
+        <v>258</v>
+      </c>
+      <c r="G36" s="45">
+        <v>43</v>
+      </c>
+      <c r="H36" s="45">
+        <v>8</v>
+      </c>
+      <c r="I36" s="45">
+        <v>13</v>
+      </c>
+      <c r="J36" s="45">
+        <v>1</v>
+      </c>
+      <c r="K36" s="45">
+        <v>4</v>
+      </c>
+      <c r="L36" s="45">
+        <v>5</v>
+      </c>
+      <c r="M36" s="45">
+        <v>2</v>
+      </c>
+      <c r="N36" s="45">
+        <v>9</v>
+      </c>
+      <c r="O36" s="45">
+        <v>3</v>
+      </c>
+      <c r="P36" s="45">
+        <v>1</v>
+      </c>
+      <c r="Q36" s="46">
+        <v>12</v>
+      </c>
       <c r="R36" s="40"/>
       <c r="S36" s="40"/>
       <c r="T36" s="40"/>
@@ -35329,21 +35479,51 @@
       <c r="B42" s="48" t="s">
         <v>53</v>
       </c>
-      <c r="C42" s="49"/>
-      <c r="D42" s="44"/>
-      <c r="E42" s="45"/>
-      <c r="F42" s="45"/>
-      <c r="G42" s="45"/>
-      <c r="H42" s="45"/>
-      <c r="I42" s="45"/>
-      <c r="J42" s="45"/>
-      <c r="K42" s="45"/>
-      <c r="L42" s="45"/>
-      <c r="M42" s="45"/>
-      <c r="N42" s="45"/>
-      <c r="O42" s="45"/>
-      <c r="P42" s="45"/>
-      <c r="Q42" s="46"/>
+      <c r="C42" s="49">
+        <v>1</v>
+      </c>
+      <c r="D42" s="44">
+        <v>2</v>
+      </c>
+      <c r="E42" s="45">
+        <v>1</v>
+      </c>
+      <c r="F42" s="45">
+        <v>258</v>
+      </c>
+      <c r="G42" s="45">
+        <v>43</v>
+      </c>
+      <c r="H42" s="45">
+        <v>8</v>
+      </c>
+      <c r="I42" s="45">
+        <v>13</v>
+      </c>
+      <c r="J42" s="45">
+        <v>1</v>
+      </c>
+      <c r="K42" s="45">
+        <v>4</v>
+      </c>
+      <c r="L42" s="45">
+        <v>5</v>
+      </c>
+      <c r="M42" s="45">
+        <v>2</v>
+      </c>
+      <c r="N42" s="45">
+        <v>9</v>
+      </c>
+      <c r="O42" s="45">
+        <v>3</v>
+      </c>
+      <c r="P42" s="45">
+        <v>1</v>
+      </c>
+      <c r="Q42" s="46">
+        <v>12</v>
+      </c>
       <c r="R42" s="71" t="s">
         <v>54</v>
       </c>
@@ -35752,11 +35932,15 @@
     <row r="8" spans="2:27" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="13"/>
       <c r="C8" s="14"/>
-      <c r="D8" s="15"/>
+      <c r="D8" s="15">
+        <v>2</v>
+      </c>
       <c r="E8" s="15"/>
       <c r="F8" s="15"/>
       <c r="G8" s="15"/>
-      <c r="H8" s="15"/>
+      <c r="H8" s="15" t="s">
+        <v>84</v>
+      </c>
       <c r="I8" s="15"/>
       <c r="J8" s="15"/>
       <c r="K8" s="15"/>
@@ -35768,9 +35952,13 @@
       <c r="Q8" s="15"/>
       <c r="R8" s="15"/>
       <c r="S8" s="15"/>
-      <c r="T8" s="15"/>
+      <c r="T8" s="15">
+        <v>2</v>
+      </c>
       <c r="U8" s="62"/>
-      <c r="V8" s="16"/>
+      <c r="V8" s="16">
+        <v>2</v>
+      </c>
     </row>
     <row r="9" spans="2:27" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="13" t="s">
@@ -35919,11 +36107,15 @@
         <v>25</v>
       </c>
       <c r="C15" s="23"/>
-      <c r="D15" s="24"/>
+      <c r="D15" s="24">
+        <v>2</v>
+      </c>
       <c r="E15" s="24"/>
       <c r="F15" s="24"/>
       <c r="G15" s="24"/>
-      <c r="H15" s="24"/>
+      <c r="H15" s="24" t="s">
+        <v>83</v>
+      </c>
       <c r="I15" s="24"/>
       <c r="J15" s="24"/>
       <c r="K15" s="24"/>
@@ -35935,20 +36127,28 @@
       <c r="Q15" s="24"/>
       <c r="R15" s="24"/>
       <c r="S15" s="24"/>
-      <c r="T15" s="24"/>
+      <c r="T15" s="24">
+        <v>2</v>
+      </c>
       <c r="U15" s="64"/>
-      <c r="V15" s="25"/>
+      <c r="V15" s="25">
+        <v>2</v>
+      </c>
     </row>
     <row r="16" spans="2:27" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B16" s="26" t="s">
         <v>26</v>
       </c>
       <c r="C16" s="60"/>
-      <c r="D16" s="61"/>
+      <c r="D16" s="61">
+        <v>0</v>
+      </c>
       <c r="E16" s="28"/>
       <c r="F16" s="28"/>
       <c r="G16" s="29"/>
-      <c r="H16" s="29"/>
+      <c r="H16" s="29" t="s">
+        <v>82</v>
+      </c>
       <c r="I16" s="29"/>
       <c r="J16" s="29"/>
       <c r="K16" s="59"/>
@@ -35960,9 +36160,13 @@
       <c r="Q16" s="29"/>
       <c r="R16" s="29"/>
       <c r="S16" s="29"/>
-      <c r="T16" s="59"/>
+      <c r="T16" s="59">
+        <v>0</v>
+      </c>
       <c r="U16" s="65"/>
-      <c r="V16" s="30"/>
+      <c r="V16" s="30">
+        <v>0</v>
+      </c>
     </row>
     <row r="17" spans="2:22" s="5" customFormat="1" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B17" s="31"/>
@@ -36340,21 +36544,35 @@
       <c r="B24" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="C24" s="14"/>
+      <c r="C24" s="14">
+        <v>1</v>
+      </c>
       <c r="D24" s="15"/>
       <c r="E24" s="15"/>
       <c r="F24" s="15"/>
       <c r="G24" s="15"/>
-      <c r="H24" s="15"/>
+      <c r="H24" s="15">
+        <v>3</v>
+      </c>
       <c r="I24" s="15"/>
-      <c r="J24" s="15"/>
+      <c r="J24" s="15">
+        <v>46</v>
+      </c>
       <c r="K24" s="15"/>
-      <c r="L24" s="15"/>
-      <c r="M24" s="15"/>
-      <c r="N24" s="15"/>
+      <c r="L24" s="15">
+        <v>2</v>
+      </c>
+      <c r="M24" s="15">
+        <v>15</v>
+      </c>
+      <c r="N24" s="15">
+        <v>224</v>
+      </c>
       <c r="O24" s="15"/>
       <c r="P24" s="15"/>
-      <c r="Q24" s="15"/>
+      <c r="Q24" s="15">
+        <v>15</v>
+      </c>
       <c r="R24" s="15"/>
       <c r="S24" s="15"/>
       <c r="T24" s="15"/>
@@ -36505,21 +36723,35 @@
       <c r="B31" s="22" t="s">
         <v>25</v>
       </c>
-      <c r="C31" s="23"/>
+      <c r="C31" s="23">
+        <v>1</v>
+      </c>
       <c r="D31" s="24"/>
       <c r="E31" s="24"/>
       <c r="F31" s="24"/>
       <c r="G31" s="24"/>
-      <c r="H31" s="24"/>
+      <c r="H31" s="24">
+        <v>3</v>
+      </c>
       <c r="I31" s="24"/>
-      <c r="J31" s="24"/>
+      <c r="J31" s="24">
+        <v>7</v>
+      </c>
       <c r="K31" s="24"/>
-      <c r="L31" s="24"/>
-      <c r="M31" s="24"/>
-      <c r="N31" s="24"/>
+      <c r="L31" s="24">
+        <v>2</v>
+      </c>
+      <c r="M31" s="24">
+        <v>13</v>
+      </c>
+      <c r="N31" s="24">
+        <v>56</v>
+      </c>
       <c r="O31" s="24"/>
       <c r="P31" s="24"/>
-      <c r="Q31" s="24"/>
+      <c r="Q31" s="24">
+        <v>15</v>
+      </c>
       <c r="R31" s="24"/>
       <c r="S31" s="24"/>
       <c r="T31" s="24"/>
@@ -36530,21 +36762,35 @@
       <c r="B32" s="39" t="s">
         <v>26</v>
       </c>
-      <c r="C32" s="27"/>
+      <c r="C32" s="27">
+        <v>0</v>
+      </c>
       <c r="D32" s="28"/>
       <c r="E32" s="28"/>
       <c r="F32" s="28"/>
       <c r="G32" s="29"/>
-      <c r="H32" s="29"/>
+      <c r="H32" s="29">
+        <v>0</v>
+      </c>
       <c r="I32" s="29"/>
-      <c r="J32" s="29"/>
+      <c r="J32" s="29">
+        <v>39</v>
+      </c>
       <c r="K32" s="29"/>
-      <c r="L32" s="29"/>
-      <c r="M32" s="29"/>
-      <c r="N32" s="29"/>
+      <c r="L32" s="29">
+        <v>0</v>
+      </c>
+      <c r="M32" s="29">
+        <v>2</v>
+      </c>
+      <c r="N32" s="29">
+        <v>128</v>
+      </c>
       <c r="O32" s="24"/>
       <c r="P32" s="29"/>
-      <c r="Q32" s="29"/>
+      <c r="Q32" s="29">
+        <v>0</v>
+      </c>
       <c r="R32" s="29"/>
       <c r="S32" s="29"/>
       <c r="T32" s="29"/>
@@ -36673,18 +36919,36 @@
       <c r="C36" s="49"/>
       <c r="D36" s="44"/>
       <c r="E36" s="45"/>
-      <c r="F36" s="45"/>
+      <c r="F36" s="45">
+        <v>211</v>
+      </c>
       <c r="G36" s="45"/>
-      <c r="H36" s="45"/>
-      <c r="I36" s="45"/>
-      <c r="J36" s="45"/>
-      <c r="K36" s="45"/>
+      <c r="H36" s="45">
+        <v>1</v>
+      </c>
+      <c r="I36" s="45">
+        <v>2</v>
+      </c>
+      <c r="J36" s="45">
+        <v>1</v>
+      </c>
+      <c r="K36" s="45">
+        <v>8</v>
+      </c>
       <c r="L36" s="45"/>
       <c r="M36" s="45"/>
-      <c r="N36" s="45"/>
-      <c r="O36" s="45"/>
-      <c r="P36" s="45"/>
-      <c r="Q36" s="46"/>
+      <c r="N36" s="45">
+        <v>1</v>
+      </c>
+      <c r="O36" s="45">
+        <v>3</v>
+      </c>
+      <c r="P36" s="45">
+        <v>1</v>
+      </c>
+      <c r="Q36" s="46">
+        <v>22</v>
+      </c>
       <c r="R36" s="40"/>
       <c r="S36" s="40"/>
       <c r="T36" s="40"/>
@@ -36813,18 +37077,36 @@
       <c r="C42" s="49"/>
       <c r="D42" s="44"/>
       <c r="E42" s="45"/>
-      <c r="F42" s="45"/>
+      <c r="F42" s="45">
+        <v>211</v>
+      </c>
       <c r="G42" s="45"/>
-      <c r="H42" s="45"/>
-      <c r="I42" s="45"/>
-      <c r="J42" s="45"/>
-      <c r="K42" s="45"/>
+      <c r="H42" s="45">
+        <v>1</v>
+      </c>
+      <c r="I42" s="45">
+        <v>2</v>
+      </c>
+      <c r="J42" s="45">
+        <v>1</v>
+      </c>
+      <c r="K42" s="45">
+        <v>8</v>
+      </c>
       <c r="L42" s="45"/>
       <c r="M42" s="45"/>
-      <c r="N42" s="45"/>
-      <c r="O42" s="45"/>
-      <c r="P42" s="45"/>
-      <c r="Q42" s="46"/>
+      <c r="N42" s="45">
+        <v>1</v>
+      </c>
+      <c r="O42" s="45">
+        <v>3</v>
+      </c>
+      <c r="P42" s="45">
+        <v>1</v>
+      </c>
+      <c r="Q42" s="46">
+        <v>22</v>
+      </c>
       <c r="R42" s="71" t="s">
         <v>54</v>
       </c>
@@ -36879,7 +37161,7 @@
   <dimension ref="B1:AA43"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="C36" sqref="C36:Q42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
@@ -37233,11 +37515,15 @@
     <row r="8" spans="2:27" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="13"/>
       <c r="C8" s="14"/>
-      <c r="D8" s="15"/>
+      <c r="D8" s="15">
+        <v>2</v>
+      </c>
       <c r="E8" s="15"/>
       <c r="F8" s="15"/>
       <c r="G8" s="15"/>
-      <c r="H8" s="15"/>
+      <c r="H8" s="15" t="s">
+        <v>75</v>
+      </c>
       <c r="I8" s="15"/>
       <c r="J8" s="15"/>
       <c r="K8" s="15"/>
@@ -37247,11 +37533,17 @@
       <c r="O8" s="15"/>
       <c r="P8" s="15"/>
       <c r="Q8" s="15"/>
-      <c r="R8" s="15"/>
+      <c r="R8" s="15">
+        <v>9</v>
+      </c>
       <c r="S8" s="15"/>
-      <c r="T8" s="15"/>
+      <c r="T8" s="15">
+        <v>2</v>
+      </c>
       <c r="U8" s="62"/>
-      <c r="V8" s="16"/>
+      <c r="V8" s="16">
+        <v>3</v>
+      </c>
     </row>
     <row r="9" spans="2:27" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="13" t="s">
@@ -37400,11 +37692,15 @@
         <v>25</v>
       </c>
       <c r="C15" s="23"/>
-      <c r="D15" s="24"/>
+      <c r="D15" s="24">
+        <v>2</v>
+      </c>
       <c r="E15" s="24"/>
       <c r="F15" s="24"/>
       <c r="G15" s="24"/>
-      <c r="H15" s="24"/>
+      <c r="H15" s="24" t="s">
+        <v>74</v>
+      </c>
       <c r="I15" s="24"/>
       <c r="J15" s="24"/>
       <c r="K15" s="24"/>
@@ -37414,22 +37710,32 @@
       <c r="O15" s="24"/>
       <c r="P15" s="24"/>
       <c r="Q15" s="24"/>
-      <c r="R15" s="24"/>
+      <c r="R15" s="24">
+        <v>0</v>
+      </c>
       <c r="S15" s="24"/>
-      <c r="T15" s="24"/>
+      <c r="T15" s="24">
+        <v>2</v>
+      </c>
       <c r="U15" s="64"/>
-      <c r="V15" s="25"/>
+      <c r="V15" s="25">
+        <v>0</v>
+      </c>
     </row>
     <row r="16" spans="2:27" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B16" s="26" t="s">
         <v>26</v>
       </c>
       <c r="C16" s="60"/>
-      <c r="D16" s="61"/>
+      <c r="D16" s="61">
+        <v>0</v>
+      </c>
       <c r="E16" s="28"/>
       <c r="F16" s="28"/>
       <c r="G16" s="29"/>
-      <c r="H16" s="29"/>
+      <c r="H16" s="29" t="s">
+        <v>73</v>
+      </c>
       <c r="I16" s="29"/>
       <c r="J16" s="29"/>
       <c r="K16" s="59"/>
@@ -37439,11 +37745,17 @@
       <c r="O16" s="29"/>
       <c r="P16" s="29"/>
       <c r="Q16" s="29"/>
-      <c r="R16" s="29"/>
+      <c r="R16" s="29">
+        <v>9</v>
+      </c>
       <c r="S16" s="29"/>
-      <c r="T16" s="59"/>
+      <c r="T16" s="59">
+        <v>0</v>
+      </c>
       <c r="U16" s="65"/>
-      <c r="V16" s="30"/>
+      <c r="V16" s="30">
+        <v>3</v>
+      </c>
     </row>
     <row r="17" spans="2:22" s="5" customFormat="1" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B17" s="31"/>
@@ -37821,21 +38133,35 @@
       <c r="B24" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="C24" s="14"/>
+      <c r="C24" s="14">
+        <v>1</v>
+      </c>
       <c r="D24" s="15"/>
       <c r="E24" s="15"/>
       <c r="F24" s="15"/>
       <c r="G24" s="15"/>
-      <c r="H24" s="15"/>
+      <c r="H24" s="15">
+        <v>2</v>
+      </c>
       <c r="I24" s="15"/>
-      <c r="J24" s="15"/>
+      <c r="J24" s="15">
+        <v>84</v>
+      </c>
       <c r="K24" s="15"/>
-      <c r="L24" s="15"/>
-      <c r="M24" s="15"/>
-      <c r="N24" s="15"/>
+      <c r="L24" s="15">
+        <v>2</v>
+      </c>
+      <c r="M24" s="15">
+        <v>12</v>
+      </c>
+      <c r="N24" s="15">
+        <v>445</v>
+      </c>
       <c r="O24" s="15"/>
       <c r="P24" s="15"/>
-      <c r="Q24" s="15"/>
+      <c r="Q24" s="15">
+        <v>10</v>
+      </c>
       <c r="R24" s="15"/>
       <c r="S24" s="15"/>
       <c r="T24" s="15"/>
@@ -37986,21 +38312,35 @@
       <c r="B31" s="22" t="s">
         <v>25</v>
       </c>
-      <c r="C31" s="23"/>
+      <c r="C31" s="23">
+        <v>1</v>
+      </c>
       <c r="D31" s="24"/>
       <c r="E31" s="24"/>
       <c r="F31" s="24"/>
       <c r="G31" s="24"/>
-      <c r="H31" s="24"/>
+      <c r="H31" s="24">
+        <v>0</v>
+      </c>
       <c r="I31" s="24"/>
-      <c r="J31" s="24"/>
+      <c r="J31" s="24">
+        <v>66</v>
+      </c>
       <c r="K31" s="24"/>
-      <c r="L31" s="24"/>
-      <c r="M31" s="24"/>
-      <c r="N31" s="24"/>
+      <c r="L31" s="24">
+        <v>1</v>
+      </c>
+      <c r="M31" s="24">
+        <v>1</v>
+      </c>
+      <c r="N31" s="24">
+        <v>234</v>
+      </c>
       <c r="O31" s="24"/>
       <c r="P31" s="24"/>
-      <c r="Q31" s="24"/>
+      <c r="Q31" s="24">
+        <v>10</v>
+      </c>
       <c r="R31" s="24"/>
       <c r="S31" s="24"/>
       <c r="T31" s="24"/>
@@ -38011,21 +38351,35 @@
       <c r="B32" s="39" t="s">
         <v>26</v>
       </c>
-      <c r="C32" s="27"/>
+      <c r="C32" s="27">
+        <v>0</v>
+      </c>
       <c r="D32" s="28"/>
       <c r="E32" s="28"/>
       <c r="F32" s="28"/>
       <c r="G32" s="29"/>
-      <c r="H32" s="29"/>
+      <c r="H32" s="29">
+        <v>2</v>
+      </c>
       <c r="I32" s="29"/>
-      <c r="J32" s="29"/>
+      <c r="J32" s="29">
+        <v>18</v>
+      </c>
       <c r="K32" s="29"/>
-      <c r="L32" s="29"/>
-      <c r="M32" s="29"/>
-      <c r="N32" s="29"/>
+      <c r="L32" s="29">
+        <v>1</v>
+      </c>
+      <c r="M32" s="29">
+        <v>11</v>
+      </c>
+      <c r="N32" s="29">
+        <v>211</v>
+      </c>
       <c r="O32" s="24"/>
       <c r="P32" s="29"/>
-      <c r="Q32" s="29"/>
+      <c r="Q32" s="29">
+        <v>0</v>
+      </c>
       <c r="R32" s="29"/>
       <c r="S32" s="29"/>
       <c r="T32" s="29"/>
@@ -38151,21 +38505,43 @@
       <c r="B36" s="55" t="s">
         <v>52</v>
       </c>
-      <c r="C36" s="49"/>
+      <c r="C36" s="49">
+        <v>2</v>
+      </c>
       <c r="D36" s="44"/>
-      <c r="E36" s="45"/>
-      <c r="F36" s="45"/>
+      <c r="E36" s="45">
+        <v>3</v>
+      </c>
+      <c r="F36" s="45">
+        <v>262</v>
+      </c>
       <c r="G36" s="45"/>
       <c r="H36" s="45"/>
-      <c r="I36" s="45"/>
+      <c r="I36" s="45">
+        <v>10</v>
+      </c>
       <c r="J36" s="45"/>
-      <c r="K36" s="45"/>
-      <c r="L36" s="45"/>
-      <c r="M36" s="45"/>
-      <c r="N36" s="45"/>
-      <c r="O36" s="45"/>
-      <c r="P36" s="45"/>
-      <c r="Q36" s="46"/>
+      <c r="K36" s="45">
+        <v>9</v>
+      </c>
+      <c r="L36" s="45">
+        <v>2</v>
+      </c>
+      <c r="M36" s="45">
+        <v>1</v>
+      </c>
+      <c r="N36" s="45">
+        <v>11</v>
+      </c>
+      <c r="O36" s="45">
+        <v>4</v>
+      </c>
+      <c r="P36" s="45">
+        <v>1</v>
+      </c>
+      <c r="Q36" s="46">
+        <v>6</v>
+      </c>
       <c r="R36" s="40"/>
       <c r="S36" s="40"/>
       <c r="T36" s="40"/>
@@ -38291,21 +38667,43 @@
       <c r="B42" s="48" t="s">
         <v>53</v>
       </c>
-      <c r="C42" s="49"/>
+      <c r="C42" s="49">
+        <v>2</v>
+      </c>
       <c r="D42" s="44"/>
-      <c r="E42" s="45"/>
-      <c r="F42" s="45"/>
+      <c r="E42" s="45">
+        <v>3</v>
+      </c>
+      <c r="F42" s="45">
+        <v>262</v>
+      </c>
       <c r="G42" s="45"/>
       <c r="H42" s="45"/>
-      <c r="I42" s="45"/>
+      <c r="I42" s="45">
+        <v>10</v>
+      </c>
       <c r="J42" s="45"/>
-      <c r="K42" s="45"/>
-      <c r="L42" s="45"/>
-      <c r="M42" s="45"/>
-      <c r="N42" s="45"/>
-      <c r="O42" s="45"/>
-      <c r="P42" s="45"/>
-      <c r="Q42" s="46"/>
+      <c r="K42" s="45">
+        <v>9</v>
+      </c>
+      <c r="L42" s="45">
+        <v>2</v>
+      </c>
+      <c r="M42" s="45">
+        <v>1</v>
+      </c>
+      <c r="N42" s="45">
+        <v>11</v>
+      </c>
+      <c r="O42" s="45">
+        <v>4</v>
+      </c>
+      <c r="P42" s="45">
+        <v>1</v>
+      </c>
+      <c r="Q42" s="46">
+        <v>6</v>
+      </c>
       <c r="R42" s="71" t="s">
         <v>54</v>
       </c>

</xml_diff>